<commit_message>
fix renommage de la commodité mango|lime
</commit_message>
<xml_diff>
--- a/data/mango|lime-guinea-bissau/mango|lime-guinea-bissau-social.xlsx
+++ b/data/mango|lime-guinea-bissau/mango|lime-guinea-bissau-social.xlsx
@@ -59,7 +59,7 @@
     <t xml:space="preserve">Value chain:</t>
   </si>
   <si>
-    <t xml:space="preserve">mango</t>
+    <t xml:space="preserve">mango|lime</t>
   </si>
   <si>
     <t xml:space="preserve">Country :</t>
@@ -5763,10 +5763,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.247920133111481"/>
-          <c:y val="0.19212271973466"/>
-          <c:w val="0.50978527850408"/>
-          <c:h val="0.509784411276949"/>
+          <c:x val="0.247922108762764"/>
+          <c:y val="0.192138651629488"/>
+          <c:w val="0.509775983535186"/>
+          <c:h val="0.509743759847417"/>
         </c:manualLayout>
       </c:layout>
       <c:radarChart>
@@ -6004,13 +6004,13 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="74417547"/>
-        <c:axId val="34051491"/>
+        <c:axId val="15019371"/>
+        <c:axId val="65298285"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="74417547"/>
+        <c:axId val="15019371"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -6047,7 +6047,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34051491"/>
+        <c:crossAx val="65298285"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6055,7 +6055,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="34051491"/>
+        <c:axId val="65298285"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -6099,7 +6099,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74417547"/>
+        <c:crossAx val="15019371"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6162,9 +6162,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>299880</xdr:colOff>
+      <xdr:colOff>299520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>1240200</xdr:rowOff>
+      <xdr:rowOff>1239840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6173,7 +6173,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="6564240" y="823320"/>
-        <a:ext cx="4543200" cy="4341240"/>
+        <a:ext cx="4547520" cy="4340880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6196,16 +6196,16 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="9" min="9" style="0" width="10.85"/>
@@ -6647,7 +6647,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{B6AF56BD-DC6A-41D2-B280-7C5B153521F0}">
+          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{CB432AEE-3676-40A2-BBC3-803DD1C2BC3F}">
             <xm:f>Register!$L$6</xm:f>
             <x14:dxf>
               <fill>
@@ -6657,7 +6657,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="7" operator="equal" id="{13D04B78-B3AF-47DF-99F6-85C0FBFCCCCA}">
+          <x14:cfRule type="cellIs" priority="7" operator="equal" id="{8D39EA6F-AC2E-41DF-829E-9EB5CC458920}">
             <xm:f>Register!$L$5</xm:f>
             <x14:dxf>
               <fill>
@@ -6667,7 +6667,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="8" operator="equal" id="{E1B0F8D4-4FD7-44CC-A78A-42275660C318}">
+          <x14:cfRule type="cellIs" priority="8" operator="equal" id="{2FCA9DF0-5092-4FE3-9463-46DD2FAD2655}">
             <xm:f>Register!$L$4</xm:f>
             <x14:dxf>
               <fill>
@@ -6677,7 +6677,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="9" operator="equal" id="{2960A1A5-A343-498C-9F44-E4DCADC42AC0}">
+          <x14:cfRule type="cellIs" priority="9" operator="equal" id="{71A613F8-FC34-40CA-AE8C-9B6A99D4AAB1}">
             <xm:f>Register!$L$3</xm:f>
             <x14:dxf>
               <fill>
@@ -6708,7 +6708,7 @@
       <selection pane="bottomLeft" activeCell="H41" activeCellId="0" sqref="H41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="62" width="10.29"/>
@@ -6728,7 +6728,7 @@
     <row r="1" s="69" customFormat="true" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="63" t="str">
         <f aca="false">Profile!F1</f>
-        <v>mango</v>
+        <v>mango|lime</v>
       </c>
       <c r="B1" s="63"/>
       <c r="C1" s="64" t="s">
@@ -7915,14 +7915,14 @@
       <selection pane="bottomLeft" activeCell="D114" activeCellId="0" sqref="D114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="207" width="30.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="208" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="56" width="7.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="56" width="1.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="56" width="1.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="56" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="56" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="56" width="12.29"/>
@@ -7940,7 +7940,7 @@
       </c>
       <c r="B1" s="210" t="str">
         <f aca="false">Profile!F1</f>
-        <v>mango</v>
+        <v>mango|lime</v>
       </c>
       <c r="C1" s="64" t="s">
         <v>17</v>
@@ -11229,7 +11229,7 @@
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="126"/>

</xml_diff>